<commit_message>
additions to data model
</commit_message>
<xml_diff>
--- a/documentation/DataAndPseudoRelationships.xlsx
+++ b/documentation/DataAndPseudoRelationships.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="116">
   <si>
     <t>USER</t>
   </si>
@@ -221,12 +221,6 @@
     <t>INDOOR</t>
   </si>
   <si>
-    <t>FIELDS</t>
-  </si>
-  <si>
-    <t>{FIELD}</t>
-  </si>
-  <si>
     <t>FIELD_SIZE</t>
   </si>
   <si>
@@ -338,18 +332,6 @@
     <t>PARENT_PLAYER']</t>
   </si>
   <si>
-    <t>'RECREATIONAL',</t>
-  </si>
-  <si>
-    <t>'IN_HOUSE',</t>
-  </si>
-  <si>
-    <t>'ADULT']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['TRAVEL', </t>
-  </si>
-  <si>
     <t>['FORFEIT',</t>
   </si>
   <si>
@@ -366,6 +348,30 @@
   </si>
   <si>
     <t>CLUB_MEMBER</t>
+  </si>
+  <si>
+    <t>TEAM_PLAYERS</t>
+  </si>
+  <si>
+    <t>PLAYER</t>
+  </si>
+  <si>
+    <t>TEAM_COACHES</t>
+  </si>
+  <si>
+    <t>COACH</t>
+  </si>
+  <si>
+    <t>LEAGUE_TYPE</t>
+  </si>
+  <si>
+    <t>LEAGUE_TEAMS</t>
+  </si>
+  <si>
+    <t>FINE</t>
+  </si>
+  <si>
+    <t>numeric</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -647,45 +653,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -746,11 +713,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -839,6 +921,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -857,56 +966,59 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1222,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W59"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,57 +1368,50 @@
     <col min="24" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="M3" s="30" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="41"/>
+      <c r="M3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="S3" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="35"/>
-    </row>
-    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="41"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -1339,24 +1444,9 @@
       <c r="Q4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="U4" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="V4" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="W4" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1401,25 +1491,10 @@
       <c r="Q5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="W5" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
-        <v>81</v>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>79</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>3</v>
@@ -1450,22 +1525,13 @@
         <v>5</v>
       </c>
       <c r="P6" s="8"/>
-      <c r="Q6" s="24"/>
-      <c r="S6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="U6" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="V6" s="8"/>
-      <c r="W6" s="24"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
-        <v>82</v>
+      <c r="Q6" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>80</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>3</v>
@@ -1497,21 +1563,10 @@
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="24"/>
-      <c r="S7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="U7" s="8"/>
-      <c r="V7" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="W7" s="24"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="52" t="s">
-        <v>83</v>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>81</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>3</v>
@@ -1541,17 +1596,10 @@
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="24"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="W8" s="24"/>
-    </row>
-    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52" t="s">
-        <v>84</v>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>82</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>3</v>
@@ -1579,17 +1627,10 @@
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="24"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="W9" s="25"/>
-    </row>
-    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
-        <v>85</v>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
+        <v>83</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -1603,14 +1644,12 @@
         <v>15</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>107</v>
-      </c>
+      <c r="J10" s="12"/>
       <c r="K10" s="24"/>
       <c r="M10" s="10" t="s">
         <v>46</v>
@@ -1624,9 +1663,9 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="24"/>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52" t="s">
-        <v>86</v>
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>3</v>
@@ -1634,13 +1673,17 @@
       <c r="C11" s="21"/>
       <c r="D11" s="8"/>
       <c r="E11" s="24"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="K11" s="39"/>
+      <c r="G11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="25"/>
       <c r="M11" s="10" t="s">
         <v>47</v>
       </c>
@@ -1652,16 +1695,9 @@
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="24"/>
-      <c r="S11" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="32"/>
-    </row>
-    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="52" t="s">
+    </row>
+    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="38" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1670,13 +1706,11 @@
       <c r="C12" s="21"/>
       <c r="D12" s="8"/>
       <c r="E12" s="24"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="K12" s="39"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
       <c r="M12" s="10" t="s">
         <v>48</v>
       </c>
@@ -1686,24 +1720,9 @@
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="9"/>
-      <c r="S12" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="T12" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="U12" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="V12" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="W12" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="38" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1712,13 +1731,13 @@
       <c r="C13" s="21"/>
       <c r="D13" s="8"/>
       <c r="E13" s="24"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="K13" s="39"/>
+      <c r="G13" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41"/>
       <c r="M13" s="10" t="s">
         <v>49</v>
       </c>
@@ -1728,24 +1747,9 @@
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="9"/>
-      <c r="S13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U13" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="W13" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="52" t="s">
+    </row>
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1754,17 +1758,21 @@
       <c r="C14" s="21"/>
       <c r="D14" s="8"/>
       <c r="E14" s="24"/>
-      <c r="G14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="25"/>
+      <c r="G14" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="62" t="s">
+        <v>8</v>
+      </c>
       <c r="M14" s="10" t="s">
         <v>51</v>
       </c>
@@ -1774,23 +1782,10 @@
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="9"/>
-      <c r="S14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U14" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="V14" s="8"/>
-      <c r="W14" s="29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="52" t="s">
-        <v>87</v>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
+        <v>85</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>3</v>
@@ -1798,11 +1793,17 @@
       <c r="C15" s="21"/>
       <c r="D15" s="8"/>
       <c r="E15" s="24"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="G15" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
       <c r="M15" s="10" t="s">
         <v>52</v>
       </c>
@@ -1812,18 +1813,9 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
-      <c r="S15" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="U15" s="27"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="29"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="52" t="s">
+    </row>
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="38" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1832,13 +1824,17 @@
       <c r="C16" s="21"/>
       <c r="D16" s="8"/>
       <c r="E16" s="24"/>
-      <c r="G16" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
+      <c r="G16" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="25"/>
       <c r="M16" s="10" t="s">
         <v>53</v>
       </c>
@@ -1848,19 +1844,10 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
-      <c r="S16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="T16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="9"/>
-    </row>
-    <row r="17" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>6</v>
@@ -1870,21 +1857,6 @@
         <v>0</v>
       </c>
       <c r="E17" s="24"/>
-      <c r="G17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>8</v>
-      </c>
       <c r="M17" s="10" t="s">
         <v>54</v>
       </c>
@@ -1894,19 +1866,10 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="9"/>
-      <c r="S17" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="T17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="9"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>3</v>
@@ -1914,21 +1877,13 @@
       <c r="C18" s="21"/>
       <c r="D18" s="8"/>
       <c r="E18" s="24"/>
-      <c r="G18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="G18" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="41"/>
       <c r="M18" s="10" t="s">
         <v>55</v>
       </c>
@@ -1938,19 +1893,10 @@
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="9"/>
-      <c r="S18" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="T18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="9"/>
-    </row>
-    <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>3</v>
@@ -1958,17 +1904,21 @@
       <c r="C19" s="22"/>
       <c r="D19" s="14"/>
       <c r="E19" s="25"/>
-      <c r="G19" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="24"/>
+      <c r="G19" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="62" t="s">
+        <v>8</v>
+      </c>
       <c r="M19" s="10" t="s">
         <v>56</v>
       </c>
@@ -1978,30 +1928,23 @@
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="9"/>
-      <c r="S19" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="9"/>
-    </row>
-    <row r="20" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G20" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="24"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="59" t="s">
+        <v>5</v>
+      </c>
       <c r="M20" s="10" t="s">
         <v>57</v>
       </c>
@@ -2011,27 +1954,24 @@
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="9"/>
-      <c r="S20" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="9"/>
-    </row>
-    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="22"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+      <c r="G21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>5</v>
+      </c>
       <c r="J21" s="14"/>
       <c r="K21" s="25"/>
       <c r="M21" s="10" t="s">
@@ -2043,19 +1983,8 @@
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
-      <c r="S21" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="T21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="W21" s="15"/>
-    </row>
-    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>1</v>
       </c>
@@ -2071,6 +2000,11 @@
       <c r="E22" s="19" t="s">
         <v>8</v>
       </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="30"/>
       <c r="M22" s="10" t="s">
         <v>59</v>
       </c>
@@ -2081,9 +2015,9 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="9"/>
     </row>
-    <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>22</v>
@@ -2093,15 +2027,15 @@
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
+        <v>90</v>
+      </c>
+      <c r="G23" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
       <c r="M23" s="10" t="s">
         <v>60</v>
       </c>
@@ -2112,9 +2046,9 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="9"/>
     </row>
-    <row r="24" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>22</v>
@@ -2122,9 +2056,9 @@
       <c r="C24" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="44"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>1</v>
@@ -2151,21 +2085,27 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="40"/>
+      <c r="E25" s="30"/>
       <c r="G25" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="7"/>
+      <c r="I25" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="23" t="s">
+        <v>5</v>
+      </c>
       <c r="M25" s="10" t="s">
         <v>62</v>
       </c>
@@ -2176,23 +2116,25 @@
       <c r="P25" s="8"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="43"/>
+    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="47"/>
       <c r="G26" s="10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>5</v>
+      </c>
       <c r="J26" s="8"/>
-      <c r="K26" s="9"/>
+      <c r="K26" s="24"/>
       <c r="M26" s="10" t="s">
         <v>63</v>
       </c>
@@ -2203,7 +2145,7 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
     </row>
-    <row r="27" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>1</v>
       </c>
@@ -2220,14 +2162,18 @@
         <v>8</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="24"/>
       <c r="M27" s="10" t="s">
         <v>64</v>
       </c>
@@ -2238,7 +2184,7 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
@@ -2254,26 +2200,19 @@
       <c r="E28" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="9"/>
-      <c r="M28" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="N28" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="15"/>
-    </row>
-    <row r="29" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>13</v>
       </c>
@@ -2284,143 +2223,159 @@
         <v>5</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="M29" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="41"/>
+    </row>
+    <row r="30" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="45" t="s">
-        <v>97</v>
+      <c r="D30" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="E30" s="9"/>
-      <c r="G30" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="9"/>
-      <c r="M30" s="30" t="s">
+      <c r="G30" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="32"/>
-    </row>
-    <row r="31" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
+      <c r="M30" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q30" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="45" t="s">
-        <v>98</v>
+      <c r="D31" s="32" t="s">
+        <v>96</v>
       </c>
       <c r="E31" s="9"/>
-      <c r="G31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="9"/>
-      <c r="M31" s="17" t="s">
+      <c r="G31" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="N31" s="18" t="s">
+      <c r="H31" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="O31" s="18" t="s">
+      <c r="I31" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="P31" s="18" t="s">
+      <c r="J31" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="Q31" s="19" t="s">
+      <c r="K31" s="19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="M31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="45" t="s">
-        <v>99</v>
+      <c r="D32" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="E32" s="9"/>
-      <c r="G32" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="9"/>
-      <c r="M32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N32" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="7"/>
+      <c r="H32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="7"/>
+      <c r="M32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="45" t="s">
-        <v>100</v>
+      <c r="D33" s="32" t="s">
+        <v>98</v>
       </c>
       <c r="E33" s="9"/>
       <c r="G33" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="9"/>
       <c r="M33" s="10" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O33" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>5</v>
+      </c>
       <c r="P33" s="8"/>
-      <c r="Q33" s="9"/>
+      <c r="Q33" s="29"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="45" t="s">
-        <v>101</v>
+      <c r="D34" s="32" t="s">
+        <v>99</v>
       </c>
       <c r="E34" s="9"/>
       <c r="G34" s="10" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>21</v>
@@ -2429,25 +2384,27 @@
       <c r="J34" s="8"/>
       <c r="K34" s="9"/>
       <c r="M34" s="10" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O34" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>5</v>
+      </c>
       <c r="P34" s="8"/>
-      <c r="Q34" s="9"/>
+      <c r="Q34" s="29"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="45" t="s">
-        <v>102</v>
+      <c r="D35" s="32" t="s">
+        <v>100</v>
       </c>
       <c r="E35" s="9"/>
       <c r="G35" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>21</v>
@@ -2456,10 +2413,10 @@
       <c r="J35" s="8"/>
       <c r="K35" s="9"/>
       <c r="M35" s="10" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -2469,24 +2426,24 @@
       <c r="A36" s="13"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
-      <c r="D36" s="46" t="s">
-        <v>103</v>
+      <c r="D36" s="33" t="s">
+        <v>101</v>
       </c>
       <c r="E36" s="15"/>
       <c r="G36" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="9"/>
       <c r="M36" s="10" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
@@ -2494,46 +2451,46 @@
     </row>
     <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G37" s="10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="9"/>
       <c r="M37" s="10" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
       <c r="Q37" s="9"/>
     </row>
     <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="32"/>
+      <c r="A38" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
       <c r="G38" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="9"/>
       <c r="M38" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
@@ -2555,20 +2512,20 @@
       <c r="E39" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H39" s="14" t="s">
+      <c r="G39" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="9"/>
+      <c r="M39" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="N39" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="15"/>
-      <c r="M39" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
@@ -2591,15 +2548,26 @@
         <v>5</v>
       </c>
       <c r="F40" s="16"/>
-      <c r="M40" s="10" t="s">
+      <c r="G40" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N40" s="8" t="s">
+      <c r="H40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="9"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="9"/>
+      <c r="M40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N40" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q40" s="15"/>
     </row>
     <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
@@ -2615,192 +2583,167 @@
       <c r="E41" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="32"/>
-      <c r="M41" s="10" t="s">
+      <c r="G41" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N41" s="8" t="s">
+      <c r="H41" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="9"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A42" s="10"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="27"/>
       <c r="D42" s="8"/>
       <c r="E42" s="29"/>
-      <c r="G42" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I42" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J42" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K42" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="M42" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N42" s="8" t="s">
+      <c r="H42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="9"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="9"/>
+      <c r="M42" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="N42" s="40"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="40"/>
+      <c r="Q42" s="41"/>
+    </row>
+    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
-      <c r="G43" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="M43" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="N43" s="8" t="s">
+      <c r="H43" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="9"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="9"/>
+      <c r="M43" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N43" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O43" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q43" s="19" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A44" s="10"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="G44" s="10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" s="27" t="s">
-        <v>5</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I44" s="8"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="M44" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N44" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="M44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O44" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q44" s="28" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>21</v>
-      </c>
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="15"/>
       <c r="G45" s="10" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="H45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="9"/>
+      <c r="M45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O45" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G46" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="15"/>
+      <c r="M46" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N46" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I45" s="27"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="29"/>
-      <c r="M45" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="N45" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="9"/>
-    </row>
-    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G46" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H46" s="8" t="s">
+      <c r="O46" s="27"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="29"/>
+    </row>
+    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="41"/>
+      <c r="M47" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N47" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="9"/>
-      <c r="M46" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N46" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="15"/>
-    </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
-      <c r="G47" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="9"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="9"/>
     </row>
     <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
@@ -2818,17 +2761,24 @@
       <c r="E48" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H48" s="14" t="s">
+      <c r="G48" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="44"/>
+      <c r="M48" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="N48" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="15"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="9"/>
+    </row>
+    <row r="49" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -2844,8 +2794,32 @@
       <c r="E49" s="28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G49" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I49" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J49" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="M49" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="N49" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="15"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>13</v>
       </c>
@@ -2857,8 +2831,23 @@
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="29"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>12</v>
       </c>
@@ -2870,39 +2859,87 @@
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="29"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G51" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I51" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" s="8"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G52" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" s="8"/>
+      <c r="J52" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
-    </row>
-    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G53" s="10"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="K53" s="24"/>
+    </row>
+    <row r="54" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="15"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="32"/>
-    </row>
-    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G54" s="10"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K54" s="24"/>
+    </row>
+    <row r="55" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G55" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I55" s="14"/>
+      <c r="J55" s="22">
+        <v>0</v>
+      </c>
+      <c r="K55" s="25"/>
+    </row>
+    <row r="56" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="41"/>
+    </row>
+    <row r="57" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>1</v>
       </c>
@@ -2919,9 +2956,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>22</v>
@@ -2932,7 +2969,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="28"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>0</v>
       </c>
@@ -2945,17 +2982,126 @@
       <c r="D59" s="8"/>
       <c r="E59" s="29"/>
     </row>
+    <row r="60" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="41"/>
+    </row>
+    <row r="62" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="28"/>
+    </row>
+    <row r="64" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="14"/>
+      <c r="E64" s="49"/>
+    </row>
+    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="41"/>
+    </row>
+    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="28"/>
+    </row>
+    <row r="69" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="14"/>
+      <c r="E69" s="49"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G13:K13"/>
     <mergeCell ref="A47:E47"/>
     <mergeCell ref="A56:E56"/>
-    <mergeCell ref="S11:W11"/>
+    <mergeCell ref="M29:Q29"/>
     <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="G41:K41"/>
+    <mergeCell ref="M42:Q42"/>
+    <mergeCell ref="G30:K30"/>
     <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="G48:K48"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="A21:E21"/>

</xml_diff>

<commit_message>
added events and placeholder for ORGANIZATION
organization is missing, added placeholder
</commit_message>
<xml_diff>
--- a/documentation/DataAndPseudoRelationships.xlsx
+++ b/documentation/DataAndPseudoRelationships.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\match-aware\documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16212" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="UserEntities" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="180">
   <si>
     <t>USER</t>
   </si>
@@ -563,12 +558,15 @@
   </si>
   <si>
     <t>MOBILE</t>
+  </si>
+  <si>
+    <t>ORGANIZAZTION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1236,53 +1234,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1293,6 +1249,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1600,7 +1598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1608,71 +1606,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.5546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="17.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-      <c r="M3" s="54" t="s">
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="67"/>
+      <c r="M3" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
-    </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="67"/>
+      <c r="S3" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="67"/>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
@@ -1718,8 +1723,23 @@
       <c r="Q4" s="19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="W4" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>17</v>
       </c>
@@ -1765,8 +1785,23 @@
       <c r="Q5" s="23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>79</v>
       </c>
@@ -1803,7 +1838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>80</v>
       </c>
@@ -1838,7 +1873,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="24"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>81</v>
       </c>
@@ -1871,7 +1906,7 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="24"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>82</v>
       </c>
@@ -1902,7 +1937,7 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="24"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>83</v>
       </c>
@@ -1937,7 +1972,7 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="24"/>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="38" t="s">
         <v>84</v>
       </c>
@@ -1970,7 +2005,7 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="24"/>
     </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="38" t="s">
         <v>44</v>
       </c>
@@ -1995,7 +2030,7 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="38" t="s">
         <v>45</v>
       </c>
@@ -2005,13 +2040,13 @@
       <c r="C13" s="21"/>
       <c r="D13" s="8"/>
       <c r="E13" s="24"/>
-      <c r="G13" s="54" t="s">
+      <c r="G13" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
       <c r="M13" s="10" t="s">
         <v>49</v>
       </c>
@@ -2022,7 +2057,7 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="9"/>
     </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
         <v>46</v>
       </c>
@@ -2057,7 +2092,7 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>85</v>
       </c>
@@ -2088,7 +2123,7 @@
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
         <v>47</v>
       </c>
@@ -2119,7 +2154,7 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
     </row>
-    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>86</v>
       </c>
@@ -2141,7 +2176,7 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="9"/>
     </row>
-    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>168</v>
       </c>
@@ -2153,13 +2188,13 @@
         <v>169</v>
       </c>
       <c r="E18" s="24"/>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="67"/>
       <c r="M18" s="10" t="s">
         <v>55</v>
       </c>
@@ -2170,7 +2205,7 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="9"/>
     </row>
-    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>170</v>
       </c>
@@ -2207,7 +2242,7 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="9"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>87</v>
       </c>
@@ -2242,7 +2277,7 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="9"/>
     </row>
-    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>88</v>
       </c>
@@ -2273,7 +2308,7 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
     </row>
-    <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G22" s="16"/>
       <c r="H22" s="41"/>
       <c r="I22" s="30"/>
@@ -2289,21 +2324,21 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="9"/>
     </row>
-    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="63" t="s">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="G23" s="60" t="s">
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="70"/>
+      <c r="G23" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="62"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="73"/>
       <c r="M23" s="10" t="s">
         <v>60</v>
       </c>
@@ -2314,7 +2349,7 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="9"/>
     </row>
-    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>1</v>
       </c>
@@ -2355,7 +2390,7 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>92</v>
       </c>
@@ -2394,7 +2429,7 @@
       <c r="P25" s="8"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>93</v>
       </c>
@@ -2429,7 +2464,7 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
     </row>
-    <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2458,14 +2493,14 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="63" t="s">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="70"/>
       <c r="G28" s="13" t="s">
         <v>13</v>
       </c>
@@ -2478,7 +2513,7 @@
       <c r="J28" s="14"/>
       <c r="K28" s="25"/>
     </row>
-    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>1</v>
       </c>
@@ -2494,15 +2529,15 @@
       <c r="E29" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="54" t="s">
+      <c r="M29" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="56"/>
-    </row>
-    <row r="30" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N29" s="66"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="67"/>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
@@ -2518,13 +2553,13 @@
       <c r="E30" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="54" t="s">
+      <c r="G30" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="56"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="67"/>
       <c r="M30" s="17" t="s">
         <v>1</v>
       </c>
@@ -2541,7 +2576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>13</v>
       </c>
@@ -2588,7 +2623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2619,7 +2654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2648,7 +2683,7 @@
       <c r="P33" s="8"/>
       <c r="Q33" s="29"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2677,7 +2712,7 @@
       <c r="P34" s="8"/>
       <c r="Q34" s="29"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2704,7 +2739,7 @@
       <c r="P35" s="8"/>
       <c r="Q35" s="9"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -2731,7 +2766,7 @@
       <c r="P36" s="8"/>
       <c r="Q36" s="9"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -2758,7 +2793,7 @@
       <c r="P37" s="8"/>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2785,7 +2820,7 @@
       <c r="P38" s="8"/>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G39" s="10" t="s">
         <v>32</v>
       </c>
@@ -2805,14 +2840,14 @@
       <c r="P39" s="8"/>
       <c r="Q39" s="9"/>
     </row>
-    <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="54" t="s">
+    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="55"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="56"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="67"/>
       <c r="F40" s="16"/>
       <c r="G40" s="10" t="s">
         <v>33</v>
@@ -2835,7 +2870,7 @@
       </c>
       <c r="Q40" s="15"/>
     </row>
-    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>1</v>
       </c>
@@ -2861,7 +2896,7 @@
       <c r="J41" s="8"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>17</v>
       </c>
@@ -2886,15 +2921,15 @@
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="9"/>
-      <c r="M42" s="54" t="s">
+      <c r="M42" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="N42" s="55"/>
-      <c r="O42" s="55"/>
-      <c r="P42" s="55"/>
-      <c r="Q42" s="56"/>
-    </row>
-    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N42" s="66"/>
+      <c r="O42" s="66"/>
+      <c r="P42" s="66"/>
+      <c r="Q42" s="67"/>
+    </row>
+    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>13</v>
       </c>
@@ -2933,7 +2968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="8"/>
       <c r="C44" s="27"/>
@@ -2964,7 +2999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -2993,7 +3028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3018,7 +3053,7 @@
       <c r="P46" s="8"/>
       <c r="Q46" s="29"/>
     </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -3034,14 +3069,14 @@
       <c r="P47" s="8"/>
       <c r="Q47" s="9"/>
     </row>
-    <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G48" s="57" t="s">
+    <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G48" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="59"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="64"/>
       <c r="M48" s="10" t="s">
         <v>68</v>
       </c>
@@ -3052,14 +3087,14 @@
       <c r="P48" s="8"/>
       <c r="Q48" s="9"/>
     </row>
-    <row r="49" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="54" t="s">
+    <row r="49" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="56"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="67"/>
       <c r="G49" s="17" t="s">
         <v>1</v>
       </c>
@@ -3085,7 +3120,7 @@
       <c r="P49" s="14"/>
       <c r="Q49" s="15"/>
     </row>
-    <row r="50" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
         <v>1</v>
       </c>
@@ -3117,7 +3152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>17</v>
       </c>
@@ -3145,7 +3180,7 @@
       <c r="J51" s="8"/>
       <c r="K51" s="24"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>13</v>
       </c>
@@ -3169,7 +3204,7 @@
       </c>
       <c r="K52" s="24"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>12</v>
       </c>
@@ -3189,7 +3224,7 @@
       </c>
       <c r="K53" s="24"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -3203,7 +3238,7 @@
       </c>
       <c r="K54" s="24"/>
     </row>
-    <row r="55" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="10"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -3221,30 +3256,30 @@
       </c>
       <c r="K55" s="25"/>
     </row>
-    <row r="56" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="15"/>
     </row>
-    <row r="57" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G57" s="57" t="s">
+    <row r="57" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G57" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="59"/>
-    </row>
-    <row r="58" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="54" t="s">
+      <c r="H57" s="63"/>
+      <c r="I57" s="63"/>
+      <c r="J57" s="63"/>
+      <c r="K57" s="64"/>
+    </row>
+    <row r="58" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="56"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="67"/>
       <c r="G58" s="17" t="s">
         <v>1</v>
       </c>
@@ -3261,7 +3296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>1</v>
       </c>
@@ -3293,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>106</v>
       </c>
@@ -3317,7 +3352,7 @@
       <c r="J60" s="8"/>
       <c r="K60" s="24"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>0</v>
       </c>
@@ -3341,7 +3376,7 @@
       <c r="J61" s="8"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G62" s="10" t="s">
         <v>94</v>
       </c>
@@ -3354,14 +3389,14 @@
       <c r="J62" s="8"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="54" t="s">
+    <row r="63" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="55"/>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="56"/>
+      <c r="B63" s="66"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="67"/>
       <c r="G63" s="10" t="s">
         <v>105</v>
       </c>
@@ -3372,7 +3407,7 @@
       <c r="J63" s="8"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>1</v>
       </c>
@@ -3400,7 +3435,7 @@
       </c>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>105</v>
       </c>
@@ -3424,7 +3459,7 @@
       </c>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>109</v>
       </c>
@@ -3437,17 +3472,17 @@
       <c r="D66" s="14"/>
       <c r="E66" s="40"/>
     </row>
-    <row r="67" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="54" t="s">
+    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="56"/>
-    </row>
-    <row r="69" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="66"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="67"/>
+    </row>
+    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>1</v>
       </c>
@@ -3464,7 +3499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>105</v>
       </c>
@@ -3477,7 +3512,7 @@
       <c r="D70" s="6"/>
       <c r="E70" s="28"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
         <v>111</v>
       </c>
@@ -3491,17 +3526,8 @@
       <c r="E71" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="M29:Q29"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="M42:Q42"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G23:K23"/>
+  <mergeCells count="19">
+    <mergeCell ref="S3:W3"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A68:E68"/>
     <mergeCell ref="G18:K18"/>
@@ -3510,6 +3536,16 @@
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="G48:K48"/>
     <mergeCell ref="G57:K57"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="M42:Q42"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A40:E40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3520,31 +3556,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -3561,7 +3597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -3578,7 +3614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -3591,7 +3627,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>106</v>
       </c>
@@ -3604,7 +3640,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>94</v>
       </c>
@@ -3617,7 +3653,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>105</v>
       </c>
@@ -3628,7 +3664,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>117</v>
       </c>
@@ -3641,7 +3677,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>119</v>
       </c>
@@ -3654,17 +3690,17 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="57" t="s">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>1</v>
       </c>
@@ -3681,7 +3717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -3698,7 +3734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
@@ -3716,17 +3752,17 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="57" t="s">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="64"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
@@ -3743,7 +3779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -3760,7 +3796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
@@ -3771,7 +3807,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>15</v>
       </c>
@@ -3784,7 +3820,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>125</v>
       </c>
@@ -3795,7 +3831,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>124</v>
       </c>
@@ -3806,7 +3842,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="24"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
@@ -3817,7 +3853,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="24"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>129</v>
       </c>
@@ -3831,7 +3867,7 @@
       <c r="E24" s="24"/>
       <c r="I24" s="52"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>14</v>
       </c>
@@ -3842,7 +3878,7 @@
       <c r="D25" s="8"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
@@ -3853,7 +3889,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>143</v>
       </c>
@@ -3864,7 +3900,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>144</v>
       </c>
@@ -3875,7 +3911,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>128</v>
       </c>
@@ -3886,7 +3922,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="24"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>145</v>
       </c>
@@ -3897,7 +3933,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>70</v>
       </c>
@@ -3908,7 +3944,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>158</v>
       </c>
@@ -3919,7 +3955,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="24"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>126</v>
       </c>
@@ -3930,7 +3966,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="24"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>119</v>
       </c>
@@ -3946,18 +3982,18 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="74" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="75"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="55"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="61"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>146</v>
       </c>
@@ -3970,23 +4006,23 @@
       </c>
       <c r="E36" s="25"/>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="30"/>
       <c r="D37" s="16"/>
       <c r="E37" s="30"/>
     </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="57" t="s">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="59"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="64"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>1</v>
       </c>
@@ -4003,7 +4039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -4020,7 +4056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>153</v>
       </c>
@@ -4033,7 +4069,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>154</v>
       </c>
@@ -4046,33 +4082,33 @@
       <c r="D42" s="8"/>
       <c r="E42" s="24"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="74" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="67"/>
-      <c r="D43" s="66" t="s">
+      <c r="C43" s="55"/>
+      <c r="D43" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="75"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="74" t="s">
+      <c r="E43" s="61"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="B44" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="66"/>
-      <c r="E44" s="75"/>
-    </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="54"/>
+      <c r="E44" s="61"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>155</v>
       </c>
@@ -4088,17 +4124,17 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="57" t="s">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="59"/>
-    </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>1</v>
       </c>
@@ -4115,7 +4151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -4132,7 +4168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>119</v>
       </c>
@@ -4147,7 +4183,7 @@
       </c>
       <c r="E50" s="24"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>15</v>
       </c>
@@ -4162,7 +4198,7 @@
       </c>
       <c r="E51" s="24"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>122</v>
       </c>
@@ -4173,7 +4209,7 @@
       <c r="D52" s="8"/>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>163</v>
       </c>
@@ -4182,7 +4218,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>160</v>
       </c>
@@ -4193,7 +4229,7 @@
       <c r="D54" s="8"/>
       <c r="E54" s="24"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>161</v>
       </c>
@@ -4204,7 +4240,7 @@
       <c r="D55" s="8"/>
       <c r="E55" s="24"/>
     </row>
-    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>162</v>
       </c>
@@ -4215,17 +4251,17 @@
       <c r="D56" s="14"/>
       <c r="E56" s="25"/>
     </row>
-    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="57" t="s">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="59"/>
-    </row>
-    <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="64"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>1</v>
       </c>
@@ -4242,7 +4278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>17</v>
       </c>
@@ -4259,7 +4295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>122</v>
       </c>
@@ -4270,7 +4306,7 @@
       <c r="D61" s="8"/>
       <c r="E61" s="24"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>163</v>
       </c>
@@ -4281,7 +4317,7 @@
       <c r="D62" s="8"/>
       <c r="E62" s="24"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>161</v>
       </c>
@@ -4292,7 +4328,7 @@
       <c r="D63" s="8"/>
       <c r="E63" s="24"/>
     </row>
-    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>162</v>
       </c>
@@ -4303,17 +4339,17 @@
       <c r="D64" s="14"/>
       <c r="E64" s="25"/>
     </row>
-    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="63" t="s">
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="65"/>
-    </row>
-    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="69"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="70"/>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="48" t="s">
         <v>1</v>
       </c>
@@ -4330,7 +4366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>17</v>
       </c>
@@ -4347,7 +4383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>0</v>
       </c>
@@ -4358,7 +4394,7 @@
       <c r="D69" s="8"/>
       <c r="E69" s="24"/>
     </row>
-    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
         <v>173</v>
       </c>
@@ -4371,17 +4407,17 @@
       </c>
       <c r="E70" s="25"/>
     </row>
-    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="63" t="s">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="B72" s="64"/>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="65"/>
-    </row>
-    <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="69"/>
+      <c r="C72" s="69"/>
+      <c r="D72" s="69"/>
+      <c r="E72" s="70"/>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
         <v>1</v>
       </c>
@@ -4398,7 +4434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>17</v>
       </c>
@@ -4415,7 +4451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>175</v>
       </c>
@@ -4428,7 +4464,7 @@
       <c r="D75" s="8"/>
       <c r="E75" s="24"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>177</v>
       </c>
@@ -4439,7 +4475,7 @@
       <c r="D76" s="8"/>
       <c r="E76" s="24"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>178</v>
       </c>
@@ -4450,7 +4486,7 @@
       <c r="D77" s="8"/>
       <c r="E77" s="24"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>94</v>
       </c>
@@ -4463,7 +4499,7 @@
       <c r="D78" s="8"/>
       <c r="E78" s="24"/>
     </row>
-    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
         <v>119</v>
       </c>
@@ -4482,14 +4518,14 @@
     <sortCondition ref="A21:A36"/>
   </sortState>
   <mergeCells count="8">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A66:E66"/>
     <mergeCell ref="A72:E72"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4504,73 +4540,73 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="69"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="B1" s="75"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="57" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="57" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="70" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="57" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="57" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="57" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="57" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="72" t="s">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="59" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completion of data modeling
</commit_message>
<xml_diff>
--- a/documentation/DataAndPseudoRelationships.xlsx
+++ b/documentation/DataAndPseudoRelationships.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="181">
   <si>
     <t>USER</t>
   </si>
@@ -59,9 +59,6 @@
     <t>MIN_AGE_GROUP</t>
   </si>
   <si>
-    <t>ABBREVIATION</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t>EVENT</t>
   </si>
   <si>
-    <t>LEAGUE_GAME, SCRIMMAGE, TRAINING, PRACTICE, CLINIC, CAMP</t>
-  </si>
-  <si>
     <t>HOME_TEAM</t>
   </si>
   <si>
@@ -449,9 +443,6 @@
     <t>original game time has pending change request</t>
   </si>
   <si>
-    <t>[see next tab]</t>
-  </si>
-  <si>
     <t>ORGANIZATION</t>
   </si>
   <si>
@@ -515,9 +506,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>MESSAGE</t>
-  </si>
-  <si>
     <t>[_id]</t>
   </si>
   <si>
@@ -545,9 +533,6 @@
     <t>SCHEDULE_VIEW_RANGE</t>
   </si>
   <si>
-    <t>USER_INVITE</t>
-  </si>
-  <si>
     <t>INVITE_KEY</t>
   </si>
   <si>
@@ -561,6 +546,24 @@
   </si>
   <si>
     <t>ORGANIZAZTION</t>
+  </si>
+  <si>
+    <t>SHORT_NAME</t>
+  </si>
+  <si>
+    <t>ADMINISTRATOR</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>CLUB_AFFILIATION</t>
+  </si>
+  <si>
+    <t>MESSAGES</t>
+  </si>
+  <si>
+    <t>USER_INVITES</t>
   </si>
 </sst>
 </file>
@@ -1250,6 +1253,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,13 +1271,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1275,15 +1287,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1598,7 +1601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1608,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,50 +1635,50 @@
     <col min="16" max="16" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2.5703125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="67"/>
-      <c r="M3" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="67"/>
-      <c r="S3" s="65" t="s">
-        <v>179</v>
-      </c>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
-      <c r="W3" s="67"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="64"/>
+      <c r="M3" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="64"/>
+      <c r="S3" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="64"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
@@ -1741,61 +1744,61 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="K5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="Q5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="U5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="W5" s="23" t="s">
         <v>5</v>
@@ -1803,7 +1806,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>3</v>
@@ -1814,7 +1817,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="24"/>
       <c r="G6" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>3</v>
@@ -1825,7 +1828,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="24"/>
       <c r="M6" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N6" s="11" t="s">
         <v>3</v>
@@ -1837,10 +1840,21 @@
       <c r="Q6" s="24" t="s">
         <v>5</v>
       </c>
+      <c r="S6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="8"/>
+      <c r="W6" s="24"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>3</v>
@@ -1851,7 +1865,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="24"/>
       <c r="G7" s="10" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>3</v>
@@ -1862,7 +1876,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="24"/>
       <c r="M7" s="10" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>3</v>
@@ -1872,10 +1886,19 @@
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="24"/>
+      <c r="S7" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="21"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="24"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>3</v>
@@ -1889,13 +1912,13 @@
         <v>11</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="8"/>
       <c r="K8" s="24"/>
       <c r="M8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N8" s="8" t="s">
         <v>3</v>
@@ -1905,10 +1928,19 @@
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="24"/>
+      <c r="S8" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U8" s="21"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="24"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>3</v>
@@ -1917,16 +1949,16 @@
       <c r="D9" s="8"/>
       <c r="E9" s="24"/>
       <c r="G9" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="8"/>
       <c r="K9" s="24"/>
       <c r="M9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>3</v>
@@ -1936,10 +1968,19 @@
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="24"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S9" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="U9" s="21"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="24"/>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -1950,10 +1991,10 @@
       <c r="D10" s="8"/>
       <c r="E10" s="24"/>
       <c r="G10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>5</v>
@@ -1961,7 +2002,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="24"/>
       <c r="M10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>3</v>
@@ -1971,10 +2012,19 @@
       </c>
       <c r="P10" s="12"/>
       <c r="Q10" s="24"/>
+      <c r="S10" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="T10" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="U10" s="22"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="25"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>3</v>
@@ -1983,10 +2033,10 @@
       <c r="D11" s="8"/>
       <c r="E11" s="24"/>
       <c r="G11" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>5</v>
@@ -1994,7 +2044,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="25"/>
       <c r="M11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>3</v>
@@ -2004,10 +2054,12 @@
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="24"/>
+      <c r="U11" s="51"/>
+      <c r="W11" s="51"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>3</v>
@@ -2021,7 +2073,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="M12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>3</v>
@@ -2029,10 +2081,12 @@
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="9"/>
+      <c r="U12" s="51"/>
+      <c r="W12" s="51"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>3</v>
@@ -2040,26 +2094,28 @@
       <c r="C13" s="21"/>
       <c r="D13" s="8"/>
       <c r="E13" s="24"/>
-      <c r="G13" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="67"/>
+      <c r="G13" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
       <c r="M13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N13" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="9"/>
+      <c r="U13" s="51"/>
+      <c r="W13" s="51"/>
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>3</v>
@@ -2083,18 +2139,20 @@
         <v>8</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="9"/>
+      <c r="U14" s="51"/>
+      <c r="W14" s="51"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>3</v>
@@ -2106,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I15" s="45" t="s">
         <v>5</v>
@@ -2114,18 +2172,20 @@
       <c r="J15" s="46"/>
       <c r="K15" s="47"/>
       <c r="M15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
+      <c r="U15" s="51"/>
+      <c r="W15" s="51"/>
     </row>
     <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>3</v>
@@ -2134,10 +2194,10 @@
       <c r="D16" s="8"/>
       <c r="E16" s="24"/>
       <c r="G16" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H16" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>5</v>
@@ -2145,18 +2205,20 @@
       <c r="J16" s="14"/>
       <c r="K16" s="25"/>
       <c r="M16" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U16" s="51"/>
+      <c r="W16" s="51"/>
+    </row>
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>6</v>
@@ -2167,54 +2229,58 @@
       </c>
       <c r="E17" s="24"/>
       <c r="M17" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="9"/>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U17" s="51"/>
+      <c r="W17" s="51"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E18" s="24"/>
-      <c r="G18" s="65" t="s">
-        <v>112</v>
-      </c>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="67"/>
+      <c r="G18" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="64"/>
       <c r="M18" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="9"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U18" s="51"/>
+      <c r="W18" s="51"/>
+    </row>
+    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E19" s="24"/>
       <c r="G19" s="48" t="s">
@@ -2233,18 +2299,20 @@
         <v>8</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="9"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U19" s="51"/>
+      <c r="W19" s="51"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>3</v>
@@ -2253,33 +2321,35 @@
       <c r="D20" s="8"/>
       <c r="E20" s="24"/>
       <c r="G20" s="43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" s="46" t="s">
-        <v>23</v>
-      </c>
       <c r="K20" s="47" t="s">
         <v>5</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="9"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U20" s="51"/>
+      <c r="W20" s="51"/>
+    </row>
+    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>3</v>
@@ -2288,7 +2358,7 @@
       <c r="D21" s="14"/>
       <c r="E21" s="25"/>
       <c r="G21" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="42" t="s">
         <v>3</v>
@@ -2299,57 +2369,63 @@
       <c r="J21" s="14"/>
       <c r="K21" s="25"/>
       <c r="M21" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U21" s="51"/>
+      <c r="W21" s="51"/>
+    </row>
+    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G22" s="16"/>
       <c r="H22" s="41"/>
       <c r="I22" s="30"/>
       <c r="J22" s="16"/>
       <c r="K22" s="30"/>
       <c r="M22" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="9"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
-      <c r="G23" s="71" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="73"/>
+      <c r="U22" s="51"/>
+      <c r="W22" s="51"/>
+    </row>
+    <row r="23" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
+      <c r="G23" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="70"/>
       <c r="M23" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="9"/>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="51"/>
+      <c r="W23" s="51"/>
+    </row>
+    <row r="24" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>1</v>
       </c>
@@ -2381,70 +2457,74 @@
         <v>8</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="9"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U24" s="51"/>
+      <c r="W24" s="51"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="K25" s="23" t="s">
         <v>5</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="9"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U25" s="51"/>
+      <c r="W25" s="51"/>
+    </row>
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="31"/>
       <c r="E26" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>3</v>
@@ -2455,36 +2535,38 @@
       <c r="J26" s="8"/>
       <c r="K26" s="24"/>
       <c r="M26" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U26" s="51"/>
+      <c r="W26" s="51"/>
+    </row>
+    <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="30"/>
       <c r="G27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="K27" s="24"/>
       <c r="M27" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N27" s="8" t="s">
         <v>6</v>
@@ -2492,17 +2574,18 @@
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="70"/>
+      <c r="W27" s="51"/>
+    </row>
+    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="73"/>
       <c r="G28" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" s="14" t="s">
         <v>3</v>
@@ -2512,8 +2595,9 @@
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="25"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W28" s="51"/>
+    </row>
+    <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>1</v>
       </c>
@@ -2529,37 +2613,38 @@
       <c r="E29" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="N29" s="66"/>
-      <c r="O29" s="66"/>
-      <c r="P29" s="66"/>
-      <c r="Q29" s="67"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M29" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="64"/>
+      <c r="W29" s="51"/>
+    </row>
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E30" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="67"/>
+      <c r="G30" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="64"/>
       <c r="M30" s="17" t="s">
         <v>1</v>
       </c>
@@ -2576,9 +2661,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>3</v>
@@ -2587,10 +2672,10 @@
         <v>5</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>1</v>
@@ -2608,40 +2693,40 @@
         <v>8</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O31" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="Q31" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="9"/>
       <c r="G32" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="7"/>
       <c r="M32" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N32" s="8" t="s">
         <v>3</v>
@@ -2659,23 +2744,23 @@
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="9"/>
       <c r="G33" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="9"/>
       <c r="M33" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O33" s="27" t="s">
         <v>5</v>
@@ -2688,23 +2773,23 @@
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="9"/>
       <c r="G34" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="9"/>
       <c r="M34" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O34" s="27" t="s">
         <v>5</v>
@@ -2717,23 +2802,23 @@
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35" s="9"/>
       <c r="G35" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="9"/>
       <c r="M35" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -2744,23 +2829,23 @@
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E36" s="9"/>
       <c r="G36" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="9"/>
       <c r="M36" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
@@ -2771,23 +2856,23 @@
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E37" s="9"/>
       <c r="G37" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="9"/>
       <c r="M37" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
@@ -2798,23 +2883,23 @@
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
       <c r="D38" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E38" s="15"/>
       <c r="G38" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="9"/>
       <c r="M38" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
@@ -2822,51 +2907,51 @@
     </row>
     <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G39" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="9"/>
       <c r="M39" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="9"/>
     </row>
     <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="67"/>
+      <c r="A40" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="64"/>
       <c r="F40" s="16"/>
       <c r="G40" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="9"/>
       <c r="M40" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N40" s="14" t="s">
         <v>9</v>
       </c>
       <c r="O40" s="14"/>
       <c r="P40" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q40" s="15"/>
     </row>
@@ -2887,10 +2972,10 @@
         <v>8</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
@@ -2898,40 +2983,40 @@
     </row>
     <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E42" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="9"/>
-      <c r="M42" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="N42" s="66"/>
-      <c r="O42" s="66"/>
-      <c r="P42" s="66"/>
-      <c r="Q42" s="67"/>
+      <c r="M42" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="64"/>
     </row>
     <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>3</v>
@@ -2944,10 +3029,10 @@
         <v>5</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -2975,25 +3060,25 @@
       <c r="D44" s="8"/>
       <c r="E44" s="29"/>
       <c r="G44" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
       <c r="K44" s="9"/>
       <c r="M44" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O44" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P44" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="O44" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="P44" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="Q44" s="28" t="s">
         <v>5</v>
@@ -3006,16 +3091,16 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="G45" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="9"/>
       <c r="M45" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N45" s="8" t="s">
         <v>3</v>
@@ -3035,19 +3120,19 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="G46" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
       <c r="M46" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O46" s="27"/>
       <c r="P46" s="8"/>
@@ -3060,41 +3145,41 @@
       <c r="D47" s="14"/>
       <c r="E47" s="15"/>
       <c r="M47" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O47" s="8"/>
       <c r="P47" s="8"/>
       <c r="Q47" s="9"/>
     </row>
     <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
-      <c r="K48" s="64"/>
+      <c r="G48" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="66"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="66"/>
+      <c r="K48" s="67"/>
       <c r="M48" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O48" s="8"/>
       <c r="P48" s="8"/>
       <c r="Q48" s="9"/>
     </row>
     <row r="49" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="B49" s="66"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="66"/>
-      <c r="E49" s="67"/>
+      <c r="A49" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="64"/>
       <c r="G49" s="17" t="s">
         <v>1</v>
       </c>
@@ -3111,10 +3196,10 @@
         <v>8</v>
       </c>
       <c r="M49" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N49" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
@@ -3137,16 +3222,16 @@
         <v>8</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="I50" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="K50" s="23" t="s">
         <v>5</v>
@@ -3154,25 +3239,25 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E51" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I51" s="21" t="s">
         <v>5</v>
@@ -3182,7 +3267,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>3</v>
@@ -3193,20 +3278,20 @@
       <c r="D52" s="8"/>
       <c r="E52" s="29"/>
       <c r="G52" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I52" s="8"/>
       <c r="J52" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K52" s="24"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>3</v>
@@ -3220,7 +3305,7 @@
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="J53" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K53" s="24"/>
     </row>
@@ -3234,7 +3319,7 @@
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K54" s="24"/>
     </row>
@@ -3245,10 +3330,10 @@
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
       <c r="G55" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H55" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="H55" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="I55" s="14"/>
       <c r="J55" s="22">
@@ -3264,22 +3349,22 @@
       <c r="E56" s="15"/>
     </row>
     <row r="57" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G57" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="H57" s="63"/>
-      <c r="I57" s="63"/>
-      <c r="J57" s="63"/>
-      <c r="K57" s="64"/>
+      <c r="G57" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="H57" s="66"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="67"/>
     </row>
     <row r="58" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="67"/>
+      <c r="A58" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="64"/>
       <c r="G58" s="17" t="s">
         <v>1</v>
       </c>
@@ -3313,16 +3398,16 @@
         <v>8</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I59" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="I59" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="K59" s="23" t="s">
         <v>5</v>
@@ -3330,10 +3415,10 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C60" s="26" t="s">
         <v>5</v>
@@ -3344,7 +3429,7 @@
         <v>0</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I60" s="21" t="s">
         <v>5</v>
@@ -3357,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>5</v>
@@ -3365,10 +3450,10 @@
       <c r="D61" s="8"/>
       <c r="E61" s="29"/>
       <c r="G61" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I61" s="27" t="s">
         <v>5</v>
@@ -3378,10 +3463,10 @@
     </row>
     <row r="62" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G62" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I62" s="27" t="s">
         <v>5</v>
@@ -3390,18 +3475,18 @@
       <c r="K62" s="9"/>
     </row>
     <row r="63" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="B63" s="66"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="67"/>
+      <c r="A63" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="64"/>
       <c r="G63" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I63" s="27"/>
       <c r="J63" s="8"/>
@@ -3424,23 +3509,23 @@
         <v>8</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I64" s="27"/>
       <c r="J64" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K64" s="9"/>
     </row>
     <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>5</v>
@@ -3448,23 +3533,23 @@
       <c r="D65" s="6"/>
       <c r="E65" s="28"/>
       <c r="G65" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H65" s="14" t="s">
         <v>3</v>
       </c>
       <c r="I65" s="39"/>
       <c r="J65" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K65" s="15"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C66" s="39" t="s">
         <v>5</v>
@@ -3474,13 +3559,13 @@
     </row>
     <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="B68" s="66"/>
-      <c r="C68" s="66"/>
-      <c r="D68" s="66"/>
-      <c r="E68" s="67"/>
+      <c r="A68" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="63"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="64"/>
     </row>
     <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
@@ -3501,10 +3586,10 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C70" s="26" t="s">
         <v>5</v>
@@ -3514,10 +3599,10 @@
     </row>
     <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C71" s="39" t="s">
         <v>5</v>
@@ -3527,6 +3612,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A40:E40"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A68:E68"/>
@@ -3543,9 +3631,6 @@
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="G3:K3"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A40:E40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3557,28 +3642,28 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="51" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="A1" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -3599,16 +3684,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>5</v>
@@ -3619,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>5</v>
@@ -3629,10 +3714,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>5</v>
@@ -3642,10 +3727,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>5</v>
@@ -3655,10 +3740,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="8"/>
@@ -3666,39 +3751,39 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
+      <c r="A11" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
@@ -3719,16 +3804,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>5</v>
@@ -3736,7 +3821,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>3</v>
@@ -3748,19 +3833,17 @@
       <c r="E14" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="53" t="s">
-        <v>123</v>
-      </c>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="64"/>
+      <c r="A16" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
@@ -3781,16 +3864,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>5</v>
@@ -3798,7 +3881,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>3</v>
@@ -3809,10 +3892,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>5</v>
@@ -3822,10 +3905,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="8"/>
@@ -3833,10 +3916,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="8"/>
@@ -3847,7 +3930,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="8"/>
@@ -3855,24 +3938,24 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E24" s="24"/>
       <c r="I24" s="52"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="8"/>
@@ -3883,7 +3966,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="8"/>
@@ -3891,10 +3974,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="8"/>
@@ -3902,10 +3985,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="8"/>
@@ -3913,7 +3996,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>3</v>
@@ -3924,10 +4007,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="8"/>
@@ -3935,10 +4018,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="8"/>
@@ -3946,10 +4029,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="8"/>
@@ -3957,10 +4040,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="8"/>
@@ -3968,7 +4051,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>3</v>
@@ -3978,16 +4061,13 @@
         <v>9</v>
       </c>
       <c r="E34" s="24"/>
-      <c r="G34" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="60" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B35" s="54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="55"/>
       <c r="D35" s="54"/>
@@ -3995,14 +4075,14 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E36" s="25"/>
     </row>
@@ -4014,13 +4094,13 @@
       <c r="E37" s="30"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="62" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="64"/>
+      <c r="A38" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="67"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
@@ -4041,16 +4121,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
@@ -4058,10 +4138,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="21" t="s">
         <v>5</v>
@@ -4071,10 +4151,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>5</v>
@@ -4084,7 +4164,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B43" s="54" t="s">
         <v>3</v>
@@ -4097,10 +4177,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="60" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B44" s="54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" s="55" t="s">
         <v>5</v>
@@ -4110,10 +4190,10 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>5</v>
@@ -4121,18 +4201,18 @@
       <c r="D45" s="14"/>
       <c r="E45" s="25"/>
       <c r="G45" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="64"/>
+      <c r="A47" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" s="66"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="67"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
@@ -4153,16 +4233,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E49" s="23" t="s">
         <v>5</v>
@@ -4170,7 +4250,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>3</v>
@@ -4185,7 +4265,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>3</v>
@@ -4200,10 +4280,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="8"/>
@@ -4211,19 +4291,21 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="B53" s="8"/>
+        <v>160</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="C53" s="21"/>
       <c r="D53" s="8"/>
       <c r="E53" s="24"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="8"/>
@@ -4231,10 +4313,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="8"/>
@@ -4242,10 +4324,10 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C56" s="22"/>
       <c r="D56" s="14"/>
@@ -4253,13 +4335,13 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="62" t="s">
-        <v>164</v>
-      </c>
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="64"/>
+      <c r="A58" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="67"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
@@ -4280,16 +4362,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E60" s="23" t="s">
         <v>5</v>
@@ -4297,10 +4379,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="8"/>
@@ -4308,7 +4390,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>3</v>
@@ -4319,10 +4401,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C63" s="21"/>
       <c r="D63" s="8"/>
@@ -4330,10 +4412,10 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C64" s="22"/>
       <c r="D64" s="14"/>
@@ -4341,13 +4423,13 @@
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="B66" s="69"/>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
-      <c r="E66" s="70"/>
+      <c r="A66" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="72"/>
+      <c r="C66" s="72"/>
+      <c r="D66" s="72"/>
+      <c r="E66" s="73"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="48" t="s">
@@ -4368,16 +4450,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="46" t="s">
         <v>22</v>
-      </c>
-      <c r="C68" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="46" t="s">
-        <v>23</v>
       </c>
       <c r="E68" s="47" t="s">
         <v>5</v>
@@ -4388,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C69" s="21"/>
       <c r="D69" s="8"/>
@@ -4396,7 +4478,7 @@
     </row>
     <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>3</v>
@@ -4409,13 +4491,13 @@
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="68" t="s">
-        <v>174</v>
-      </c>
-      <c r="B72" s="69"/>
-      <c r="C72" s="69"/>
-      <c r="D72" s="69"/>
-      <c r="E72" s="70"/>
+      <c r="A72" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="72"/>
+      <c r="C72" s="72"/>
+      <c r="D72" s="72"/>
+      <c r="E72" s="73"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
@@ -4436,16 +4518,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B74" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E74" s="23" t="s">
         <v>5</v>
@@ -4453,10 +4535,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C75" s="21" t="s">
         <v>5</v>
@@ -4466,7 +4548,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>3</v>
@@ -4477,7 +4559,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>3</v>
@@ -4488,10 +4570,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C78" s="21" t="s">
         <v>5</v>
@@ -4501,7 +4583,7 @@
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B79" s="14" t="s">
         <v>3</v>
@@ -4518,14 +4600,14 @@
     <sortCondition ref="A21:A36"/>
   </sortState>
   <mergeCells count="8">
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A16:E16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A47:E47"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A72:E72"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4537,77 +4619,77 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="74" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>